<commit_message>
Made changes to tables and table fetcher
Made changes to tables fetcher and method used to fetch tables.
</commit_message>
<xml_diff>
--- a/Physics_Engine/Shared/Resources/tables/Sprites.xlsx
+++ b/Physics_Engine/Shared/Resources/tables/Sprites.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -35,12 +35,15 @@
     <t>ID</t>
   </si>
   <si>
+    <t>defaultZ</t>
+  </si>
+  <si>
+    <t>player</t>
+  </si>
+  <si>
     <t>p1</t>
   </si>
   <si>
-    <t>player1</t>
-  </si>
-  <si>
     <t>enemy1</t>
   </si>
   <si>
@@ -50,18 +53,6 @@
     <t>enemy2</t>
   </si>
   <si>
-    <t>platform1</t>
-  </si>
-  <si>
-    <t>platform2</t>
-  </si>
-  <si>
-    <t>p2</t>
-  </si>
-  <si>
-    <t>Moveable</t>
-  </si>
-  <si>
     <t>staircase2</t>
   </si>
   <si>
@@ -75,6 +66,36 @@
   </si>
   <si>
     <t>Solid</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>block1</t>
+  </si>
+  <si>
+    <t>block2</t>
+  </si>
+  <si>
+    <t>e2</t>
+  </si>
+  <si>
+    <t>rock1</t>
+  </si>
+  <si>
+    <t>r1</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>entity</t>
+  </si>
+  <si>
+    <t>block</t>
   </si>
 </sst>
 </file>
@@ -389,15 +410,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,97 +426,141 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
-        <v>11</v>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
original Physics_Engine project stopped working, so I migrated the code
Original Physics_Engine sln stopped functioning, I couldn't figure it out, so I just copied the code and files to a new solution called Game_Engine
</commit_message>
<xml_diff>
--- a/Physics_Engine/Shared/Resources/tables/Sprites.xlsx
+++ b/Physics_Engine/Shared/Resources/tables/Sprites.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -413,67 +413,67 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>